<commit_message>
updated Andrew B blurb.
</commit_message>
<xml_diff>
--- a/Resources/our_people_content.xlsx
+++ b/Resources/our_people_content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab47d1504c5bae9e/Desktop/Files/data science research centre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Desktop/adelaide-data-science-centre.github.io/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{85E4047C-DCC9-4DBC-B48D-30D9296D0DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5077E9-C55B-4970-B051-37EC1A625767}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7163790-CA2C-1948-A0BC-DB374127BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3245B7DB-705C-460B-AC4A-049CECB73394}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="41660" windowHeight="26140" xr2:uid="{3245B7DB-705C-460B-AC4A-049CECB73394}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,14 +188,6 @@
     <t>https://andxblack.github.io/</t>
   </si>
   <si>
-    <t>My research is based around stochastic modelling, mathematical epidemiology, evolution, probabilistic learning and Bayesian inference and Data Science. Some current projects are:
-- Mathematical modelling of the evolutionary transition from cells to multicellular life.
-- Developing inference methods to assist pandemic preparedness.
-- Quantifying the 1918 influenza pandemic.
-- New simulation methods and importance sampling algorithms for stochastic models.
-- Pseudo-marginal methods for Markov chain Monte Carlo.</t>
-  </si>
-  <si>
     <t>Dino Sejdinovic</t>
   </si>
   <si>
@@ -642,13 +634,16 @@
   </si>
   <si>
     <t>https://www.adelaide.edu.au/directory/chantelle.blachut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am a Senior Lecturer in Applied Mathematics at the University of Adelaide, where my research bridges the fields of data science and stochastic modelling. I strongly believe that most data can be better understood through the lens of a generative or mechanistic model and this informs much of my research. I have particular expertise in mathematical epidemiology and have developed new methods for fitting epidemic models to outbreak data to inform planning and decision making. Currently I am interested in how new generative ai techniques (diffusions, normalising flows) can be leveraged to create fast and flexible models for complex datasets. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1039,24 +1034,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7525E3-71DA-443D-999C-54F112EC76CF}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="86.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="86.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72.599999999999994">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="76.5">
+    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1114,7 +1109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.95">
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1134,7 +1129,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="152.25">
+    <row r="5" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1151,7 +1146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60.75">
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -1168,7 +1163,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60.75">
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1185,7 +1180,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="104.1" customHeight="1">
+    <row r="8" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -1202,7 +1197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="104.1" customHeight="1">
+    <row r="9" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1220,7 +1215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="144.94999999999999" customHeight="1">
+    <row r="10" spans="1:6" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1237,596 +1232,590 @@
         <v>48</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="101.45">
-      <c r="A11" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="101.45">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="116.1">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="72.599999999999994">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="144.94999999999999">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="130.5">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="60.75">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="29.1">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="130.5">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="101.45">
-      <c r="A21" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="87">
-      <c r="A22" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29.1">
-      <c r="A23" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="101.45">
-      <c r="A25" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="101.45">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="116.1">
-      <c r="A27" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="101.45">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="87">
-      <c r="A29" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="72.599999999999994">
-      <c r="A30" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="72.599999999999994">
-      <c r="A31" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.5">
-      <c r="A32" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="72.599999999999994">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.5">
-      <c r="A34" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45.75">
-      <c r="A35" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="116.1">
-      <c r="A36" s="4" t="s">
+      <c r="B36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="57.95">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="116.1">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="116.1">
-      <c r="A39" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="72.599999999999994">
-      <c r="A40" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="72.599999999999994">
-      <c r="A41" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="72.599999999999994">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29.1">
-      <c r="A43" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="29.1">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15"/>
-    <row r="46" spans="1:6" ht="15"/>
-    <row r="47" spans="1:6" ht="15"/>
-    <row r="49" ht="15"/>
-    <row r="51" ht="15"/>
-    <row r="53" ht="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" xr:uid="{71382610-89B9-46D1-ADC2-D368C7160340}"/>

</xml_diff>